<commit_message>
completed wldsearch and its relevant system
</commit_message>
<xml_diff>
--- a/analysis/version78-new alpha-beta.xlsx
+++ b/analysis/version78-new alpha-beta.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="0" windowWidth="25600" windowHeight="13800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
-  <si>
-    <t>both programs are depth 10/16, randoff, 21000 kn/s</t>
-  </si>
   <si>
     <t>version 77</t>
   </si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>both programs are depth 10/16, randoff, 21000 kl/s</t>
   </si>
 </sst>
 </file>
@@ -100,11 +100,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -442,104 +442,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2" customWidth="1"/>
     <col min="4" max="6" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
         <v>0</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3"/>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
         <v>0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3"/>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
         <v>489</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.69</v>
       </c>
-      <c r="C7" s="3">
-        <f>A7/B7</f>
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C50" si="0">A7/B7</f>
         <v>708.69565217391312</v>
       </c>
       <c r="D7">
         <v>144</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>0.21</v>
       </c>
-      <c r="F7" s="3">
-        <f>D7/E7</f>
+      <c r="F7" s="2">
+        <f t="shared" ref="F7:F50" si="1">D7/E7</f>
         <v>685.71428571428578</v>
       </c>
     </row>
@@ -547,21 +547,21 @@
       <c r="A8">
         <v>1170</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1.61</v>
       </c>
-      <c r="C8" s="3">
-        <f>A8/B8</f>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
         <v>726.70807453416148</v>
       </c>
       <c r="D8">
         <v>345</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>0.49</v>
       </c>
-      <c r="F8" s="3">
-        <f>D8/E8</f>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
         <v>704.08163265306121</v>
       </c>
     </row>
@@ -569,21 +569,21 @@
       <c r="A9">
         <v>2300</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>3.16</v>
       </c>
-      <c r="C9" s="3">
-        <f>A9/B9</f>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
         <v>727.84810126582272</v>
       </c>
       <c r="D9">
         <v>1130</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>1.62</v>
       </c>
-      <c r="F9" s="3">
-        <f>D9/E9</f>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
         <v>697.53086419753083</v>
       </c>
     </row>
@@ -591,21 +591,21 @@
       <c r="A10">
         <v>2280</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>3.12</v>
       </c>
-      <c r="C10" s="3">
-        <f>A10/B10</f>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
         <v>730.76923076923072</v>
       </c>
       <c r="D10">
         <v>1290</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1.82</v>
       </c>
-      <c r="F10" s="3">
-        <f>D10/E10</f>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
         <v>708.79120879120876</v>
       </c>
     </row>
@@ -613,21 +613,21 @@
       <c r="A11">
         <v>1940</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>2.63</v>
       </c>
-      <c r="C11" s="3">
-        <f>A11/B11</f>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
         <v>737.64258555133085</v>
       </c>
       <c r="D11">
         <v>1230</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>1.71</v>
       </c>
-      <c r="F11" s="3">
-        <f>D11/E11</f>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
         <v>719.29824561403507</v>
       </c>
     </row>
@@ -635,21 +635,21 @@
       <c r="A12">
         <v>1980</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>2.71</v>
       </c>
-      <c r="C12" s="3">
-        <f>A12/B12</f>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
         <v>730.62730627306269</v>
       </c>
       <c r="D12">
         <v>1230</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>1.73</v>
       </c>
-      <c r="F12" s="3">
-        <f>D12/E12</f>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
         <v>710.98265895953762</v>
       </c>
     </row>
@@ -657,21 +657,21 @@
       <c r="A13">
         <v>3270</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>4.43</v>
       </c>
-      <c r="C13" s="3">
-        <f>A13/B13</f>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
         <v>738.14898419864562</v>
       </c>
       <c r="D13">
         <v>870</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>1.22</v>
       </c>
-      <c r="F13" s="3">
-        <f>D13/E13</f>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
         <v>713.11475409836066</v>
       </c>
     </row>
@@ -679,21 +679,21 @@
       <c r="A14">
         <v>2910</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>3.96</v>
       </c>
-      <c r="C14" s="3">
-        <f>A14/B14</f>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
         <v>734.84848484848487</v>
       </c>
       <c r="D14">
         <v>740</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>1.05</v>
       </c>
-      <c r="F14" s="3">
-        <f>D14/E14</f>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
         <v>704.7619047619047</v>
       </c>
     </row>
@@ -701,21 +701,21 @@
       <c r="A15">
         <v>913</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>1.25</v>
       </c>
-      <c r="C15" s="3">
-        <f>A15/B15</f>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
         <v>730.4</v>
       </c>
       <c r="D15">
         <v>666</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>0.94</v>
       </c>
-      <c r="F15" s="3">
-        <f>D15/E15</f>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
         <v>708.51063829787233</v>
       </c>
     </row>
@@ -723,21 +723,21 @@
       <c r="A16">
         <v>1010</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>1.4</v>
       </c>
-      <c r="C16" s="3">
-        <f>A16/B16</f>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
         <v>721.42857142857144</v>
       </c>
       <c r="D16">
         <v>235</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>0.34</v>
       </c>
-      <c r="F16" s="3">
-        <f>D16/E16</f>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
         <v>691.17647058823525</v>
       </c>
     </row>
@@ -745,21 +745,21 @@
       <c r="A17">
         <v>2020</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>2.7</v>
       </c>
-      <c r="C17" s="3">
-        <f>A17/B17</f>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
         <v>748.14814814814815</v>
       </c>
       <c r="D17">
         <v>1850</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>2.56</v>
       </c>
-      <c r="F17" s="3">
-        <f>D17/E17</f>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
         <v>722.65625</v>
       </c>
     </row>
@@ -767,21 +767,21 @@
       <c r="A18">
         <v>2450</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>3.37</v>
       </c>
-      <c r="C18" s="3">
-        <f>A18/B18</f>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
         <v>727.00296735905044</v>
       </c>
       <c r="D18">
         <v>422</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>0.64</v>
       </c>
-      <c r="F18" s="3">
-        <f>D18/E18</f>
+      <c r="F18" s="2">
+        <f t="shared" si="1"/>
         <v>659.375</v>
       </c>
     </row>
@@ -789,21 +789,21 @@
       <c r="A19">
         <v>3640</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>4.91</v>
       </c>
-      <c r="C19" s="3">
-        <f>A19/B19</f>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
         <v>741.3441955193482</v>
       </c>
       <c r="D19">
         <v>1550</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>2.15</v>
       </c>
-      <c r="F19" s="3">
-        <f>D19/E19</f>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
         <v>720.93023255813955</v>
       </c>
     </row>
@@ -811,21 +811,21 @@
       <c r="A20">
         <v>3380</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>4.6100000000000003</v>
       </c>
-      <c r="C20" s="3">
-        <f>A20/B20</f>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
         <v>733.18872017353578</v>
       </c>
       <c r="D20">
         <v>1130</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>1.58</v>
       </c>
-      <c r="F20" s="3">
-        <f>D20/E20</f>
+      <c r="F20" s="2">
+        <f t="shared" si="1"/>
         <v>715.18987341772151</v>
       </c>
     </row>
@@ -833,21 +833,21 @@
       <c r="A21">
         <v>2770</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>3.7</v>
       </c>
-      <c r="C21" s="3">
-        <f>A21/B21</f>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
         <v>748.64864864864865</v>
       </c>
       <c r="D21">
         <v>1430</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>1.94</v>
       </c>
-      <c r="F21" s="3">
-        <f>D21/E21</f>
+      <c r="F21" s="2">
+        <f t="shared" si="1"/>
         <v>737.11340206185571</v>
       </c>
     </row>
@@ -855,21 +855,21 @@
       <c r="A22">
         <v>3490</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>4.75</v>
       </c>
-      <c r="C22" s="3">
-        <f>A22/B22</f>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
         <v>734.73684210526312</v>
       </c>
       <c r="D22">
         <v>1380</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>1.89</v>
       </c>
-      <c r="F22" s="3">
-        <f>D22/E22</f>
+      <c r="F22" s="2">
+        <f t="shared" si="1"/>
         <v>730.15873015873024</v>
       </c>
     </row>
@@ -877,21 +877,21 @@
       <c r="A23">
         <v>5690</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>7.56</v>
       </c>
-      <c r="C23" s="3">
-        <f>A23/B23</f>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
         <v>752.64550264550269</v>
       </c>
       <c r="D23">
         <v>3190</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>4.29</v>
       </c>
-      <c r="F23" s="3">
-        <f>D23/E23</f>
+      <c r="F23" s="2">
+        <f t="shared" si="1"/>
         <v>743.58974358974353</v>
       </c>
     </row>
@@ -899,21 +899,21 @@
       <c r="A24">
         <v>3010</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>4.07</v>
       </c>
-      <c r="C24" s="3">
-        <f>A24/B24</f>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
         <v>739.55773955773952</v>
       </c>
       <c r="D24">
         <v>1010</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>1.4</v>
       </c>
-      <c r="F24" s="3">
-        <f>D24/E24</f>
+      <c r="F24" s="2">
+        <f t="shared" si="1"/>
         <v>721.42857142857144</v>
       </c>
     </row>
@@ -921,21 +921,21 @@
       <c r="A25">
         <v>2390</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>3.16</v>
       </c>
-      <c r="C25" s="3">
-        <f>A25/B25</f>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
         <v>756.3291139240506</v>
       </c>
       <c r="D25">
         <v>1880</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>2.5299999999999998</v>
       </c>
-      <c r="F25" s="3">
-        <f>D25/E25</f>
+      <c r="F25" s="2">
+        <f t="shared" si="1"/>
         <v>743.08300395256924</v>
       </c>
     </row>
@@ -943,21 +943,21 @@
       <c r="A26">
         <v>2560</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>3.46</v>
       </c>
-      <c r="C26" s="3">
-        <f>A26/B26</f>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
         <v>739.88439306358384</v>
       </c>
       <c r="D26">
         <v>620</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>0.86</v>
       </c>
-      <c r="F26" s="3">
-        <f>D26/E26</f>
+      <c r="F26" s="2">
+        <f t="shared" si="1"/>
         <v>720.93023255813955</v>
       </c>
     </row>
@@ -965,21 +965,21 @@
       <c r="A27">
         <v>4590</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>6.02</v>
       </c>
-      <c r="C27" s="3">
-        <f>A27/B27</f>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
         <v>762.45847176079735</v>
       </c>
       <c r="D27">
         <v>2520</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>3.35</v>
       </c>
-      <c r="F27" s="3">
-        <f>D27/E27</f>
+      <c r="F27" s="2">
+        <f t="shared" si="1"/>
         <v>752.2388059701492</v>
       </c>
     </row>
@@ -987,21 +987,21 @@
       <c r="A28">
         <v>5160</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>6.88</v>
       </c>
-      <c r="C28" s="3">
-        <f>A28/B28</f>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
         <v>750</v>
       </c>
       <c r="D28">
         <v>1800</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>2.46</v>
       </c>
-      <c r="F28" s="3">
-        <f>D28/E28</f>
+      <c r="F28" s="2">
+        <f t="shared" si="1"/>
         <v>731.70731707317077</v>
       </c>
     </row>
@@ -1009,21 +1009,21 @@
       <c r="A29">
         <v>5320</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>6.92</v>
       </c>
-      <c r="C29" s="3">
-        <f>A29/B29</f>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
         <v>768.78612716763007</v>
       </c>
       <c r="D29">
         <v>2240</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>2.95</v>
       </c>
-      <c r="F29" s="3">
-        <f>D29/E29</f>
+      <c r="F29" s="2">
+        <f t="shared" si="1"/>
         <v>759.32203389830499</v>
       </c>
     </row>
@@ -1031,21 +1031,21 @@
       <c r="A30">
         <v>10300</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>13.93</v>
       </c>
-      <c r="C30" s="3">
-        <f>A30/B30</f>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
         <v>739.41134242641783</v>
       </c>
       <c r="D30">
         <v>4720</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>6.44</v>
       </c>
-      <c r="F30" s="3">
-        <f>D30/E30</f>
+      <c r="F30" s="2">
+        <f t="shared" si="1"/>
         <v>732.91925465838506</v>
       </c>
     </row>
@@ -1053,21 +1053,21 @@
       <c r="A31">
         <v>4630</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>6.04</v>
       </c>
-      <c r="C31" s="3">
-        <f>A31/B31</f>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
         <v>766.55629139072846</v>
       </c>
       <c r="D31">
         <v>1210</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <v>1.6</v>
       </c>
-      <c r="F31" s="3">
-        <f>D31/E31</f>
+      <c r="F31" s="2">
+        <f t="shared" si="1"/>
         <v>756.25</v>
       </c>
     </row>
@@ -1075,21 +1075,21 @@
       <c r="A32">
         <v>5470</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>7.25</v>
       </c>
-      <c r="C32" s="3">
-        <f>A32/B32</f>
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
         <v>754.48275862068965</v>
       </c>
       <c r="D32">
         <v>1890</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>2.61</v>
       </c>
-      <c r="F32" s="3">
-        <f>D32/E32</f>
+      <c r="F32" s="2">
+        <f t="shared" si="1"/>
         <v>724.13793103448279</v>
       </c>
     </row>
@@ -1097,21 +1097,21 @@
       <c r="A33">
         <v>3460</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>4.54</v>
       </c>
-      <c r="C33" s="3">
-        <f>A33/B33</f>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
         <v>762.11453744493394</v>
       </c>
       <c r="D33">
         <v>1040</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>1.38</v>
       </c>
-      <c r="F33" s="3">
-        <f>D33/E33</f>
+      <c r="F33" s="2">
+        <f t="shared" si="1"/>
         <v>753.62318840579712</v>
       </c>
     </row>
@@ -1119,21 +1119,21 @@
       <c r="A34">
         <v>5410</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>7.18</v>
       </c>
-      <c r="C34" s="3">
-        <f>A34/B34</f>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
         <v>753.48189415041782</v>
       </c>
       <c r="D34">
         <v>1470</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <v>2.0099999999999998</v>
       </c>
-      <c r="F34" s="3">
-        <f>D34/E34</f>
+      <c r="F34" s="2">
+        <f t="shared" si="1"/>
         <v>731.34328358208961</v>
       </c>
     </row>
@@ -1141,21 +1141,21 @@
       <c r="A35">
         <v>4680</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>6.12</v>
       </c>
-      <c r="C35" s="3">
-        <f>A35/B35</f>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
         <v>764.70588235294122</v>
       </c>
       <c r="D35">
         <v>1910</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="1">
         <v>2.5</v>
       </c>
-      <c r="F35" s="3">
-        <f>D35/E35</f>
+      <c r="F35" s="2">
+        <f t="shared" si="1"/>
         <v>764</v>
       </c>
     </row>
@@ -1163,21 +1163,21 @@
       <c r="A36">
         <v>5710</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>7.43</v>
       </c>
-      <c r="C36" s="3">
-        <f>A36/B36</f>
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
         <v>768.50605652759089</v>
       </c>
       <c r="D36">
         <v>2030</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="1">
         <v>2.72</v>
       </c>
-      <c r="F36" s="3">
-        <f>D36/E36</f>
+      <c r="F36" s="2">
+        <f t="shared" si="1"/>
         <v>746.32352941176464</v>
       </c>
     </row>
@@ -1185,21 +1185,21 @@
       <c r="A37">
         <v>5730</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>7.43</v>
       </c>
-      <c r="C37" s="3">
-        <f>A37/B37</f>
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
         <v>771.19784656796776</v>
       </c>
       <c r="D37">
         <v>2730</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="1">
         <v>3.53</v>
       </c>
-      <c r="F37" s="3">
-        <f>D37/E37</f>
+      <c r="F37" s="2">
+        <f t="shared" si="1"/>
         <v>773.3711048158641</v>
       </c>
     </row>
@@ -1207,21 +1207,21 @@
       <c r="A38">
         <v>3550</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>4.6399999999999997</v>
       </c>
-      <c r="C38" s="3">
-        <f>A38/B38</f>
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
         <v>765.08620689655174</v>
       </c>
       <c r="D38">
         <v>1190</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="1">
         <v>1.61</v>
       </c>
-      <c r="F38" s="3">
-        <f>D38/E38</f>
+      <c r="F38" s="2">
+        <f t="shared" si="1"/>
         <v>739.13043478260863</v>
       </c>
     </row>
@@ -1229,21 +1229,21 @@
       <c r="A39">
         <v>2250</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>2.93</v>
       </c>
-      <c r="C39" s="3">
-        <f>A39/B39</f>
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
         <v>767.91808873720129</v>
       </c>
       <c r="D39">
         <v>832</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="1">
         <v>1.08</v>
       </c>
-      <c r="F39" s="3">
-        <f>D39/E39</f>
+      <c r="F39" s="2">
+        <f t="shared" si="1"/>
         <v>770.37037037037032</v>
       </c>
     </row>
@@ -1251,21 +1251,21 @@
       <c r="A40">
         <v>2370</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>3.09</v>
       </c>
-      <c r="C40" s="3">
-        <f>A40/B40</f>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
         <v>766.990291262136</v>
       </c>
       <c r="D40">
         <v>1040</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="1">
         <v>1.39</v>
       </c>
-      <c r="F40" s="3">
-        <f>D40/E40</f>
+      <c r="F40" s="2">
+        <f t="shared" si="1"/>
         <v>748.20143884892093</v>
       </c>
     </row>
@@ -1273,21 +1273,21 @@
       <c r="A41">
         <v>1780</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>2.29</v>
       </c>
-      <c r="C41" s="3">
-        <f>A41/B41</f>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
         <v>777.29257641921402</v>
       </c>
       <c r="D41">
         <v>843</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="1">
         <v>1.0900000000000001</v>
       </c>
-      <c r="F41" s="3">
-        <f>D41/E41</f>
+      <c r="F41" s="2">
+        <f t="shared" si="1"/>
         <v>773.39449541284398</v>
       </c>
     </row>
@@ -1295,21 +1295,21 @@
       <c r="A42">
         <v>2460</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>3.22</v>
       </c>
-      <c r="C42" s="3">
-        <f>A42/B42</f>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
         <v>763.97515527950304</v>
       </c>
       <c r="D42">
         <v>542</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="1">
         <v>0.72</v>
       </c>
-      <c r="F42" s="3">
-        <f>D42/E42</f>
+      <c r="F42" s="2">
+        <f t="shared" si="1"/>
         <v>752.77777777777783</v>
       </c>
     </row>
@@ -1317,21 +1317,21 @@
       <c r="A43">
         <v>1200</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>1.56</v>
       </c>
-      <c r="C43" s="3">
-        <f>A43/B43</f>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
         <v>769.23076923076917</v>
       </c>
       <c r="D43">
         <v>498</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="1">
         <v>0.65</v>
       </c>
-      <c r="F43" s="3">
-        <f>D43/E43</f>
+      <c r="F43" s="2">
+        <f t="shared" si="1"/>
         <v>766.15384615384608</v>
       </c>
     </row>
@@ -1339,21 +1339,21 @@
       <c r="A44">
         <v>1560</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>2.06</v>
       </c>
-      <c r="C44" s="3">
-        <f>A44/B44</f>
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
         <v>757.28155339805824</v>
       </c>
       <c r="D44">
         <v>720</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="1">
         <v>0.95</v>
       </c>
-      <c r="F44" s="3">
-        <f>D44/E44</f>
+      <c r="F44" s="2">
+        <f t="shared" si="1"/>
         <v>757.89473684210532</v>
       </c>
     </row>
@@ -1361,21 +1361,21 @@
       <c r="A45">
         <v>997</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>1.3</v>
       </c>
-      <c r="C45" s="3">
-        <f>A45/B45</f>
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
         <v>766.92307692307691</v>
       </c>
       <c r="D45">
         <v>437</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F45" s="3">
-        <f>D45/E45</f>
+      <c r="F45" s="2">
+        <f t="shared" si="1"/>
         <v>766.66666666666674</v>
       </c>
     </row>
@@ -1383,21 +1383,21 @@
       <c r="A46">
         <v>598</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>0.79</v>
       </c>
-      <c r="C46" s="3">
-        <f>A46/B46</f>
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
         <v>756.96202531645565</v>
       </c>
       <c r="D46">
         <v>275</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="1">
         <v>0.37</v>
       </c>
-      <c r="F46" s="3">
-        <f>D46/E46</f>
+      <c r="F46" s="2">
+        <f t="shared" si="1"/>
         <v>743.24324324324323</v>
       </c>
     </row>
@@ -1405,21 +1405,21 @@
       <c r="A47">
         <v>343</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>0.45</v>
       </c>
-      <c r="C47" s="3">
-        <f>A47/B47</f>
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
         <v>762.22222222222217</v>
       </c>
       <c r="D47">
         <v>115</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="1">
         <v>0.15</v>
       </c>
-      <c r="F47" s="3">
-        <f>D47/E47</f>
+      <c r="F47" s="2">
+        <f t="shared" si="1"/>
         <v>766.66666666666674</v>
       </c>
     </row>
@@ -1427,21 +1427,21 @@
       <c r="A48">
         <v>257</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>0.34</v>
       </c>
-      <c r="C48" s="3">
-        <f>A48/B48</f>
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
         <v>755.88235294117646</v>
       </c>
       <c r="D48">
         <v>88.1</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="1">
         <v>0.12</v>
       </c>
-      <c r="F48" s="3">
-        <f>D48/E48</f>
+      <c r="F48" s="2">
+        <f t="shared" si="1"/>
         <v>734.16666666666663</v>
       </c>
     </row>
@@ -1449,21 +1449,21 @@
       <c r="A49">
         <v>8420</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>4.84</v>
       </c>
-      <c r="C49" s="3">
-        <f>A49/B49</f>
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
         <v>1739.6694214876034</v>
       </c>
       <c r="D49">
         <v>412</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="1">
         <v>0.43</v>
       </c>
-      <c r="F49" s="3">
-        <f>D49/E49</f>
+      <c r="F49" s="2">
+        <f t="shared" si="1"/>
         <v>958.1395348837209</v>
       </c>
     </row>
@@ -1471,21 +1471,21 @@
       <c r="A50">
         <v>3610</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>2.08</v>
       </c>
-      <c r="C50" s="3">
-        <f>A50/B50</f>
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
         <v>1735.5769230769231</v>
       </c>
       <c r="D50">
         <v>228</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="1">
         <v>0.23</v>
       </c>
-      <c r="F50" s="3">
-        <f>D50/E50</f>
+      <c r="F50" s="2">
+        <f t="shared" si="1"/>
         <v>991.30434782608688</v>
       </c>
     </row>
@@ -1493,58 +1493,58 @@
       <c r="A51">
         <v>276</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>0.17</v>
       </c>
       <c r="D51">
         <v>17.600000000000001</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="1">
         <v>0.02</v>
       </c>
-      <c r="F51" s="3"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
         <v>94.3</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D52">
         <v>11</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="1">
         <v>0.01</v>
       </c>
-      <c r="F52" s="3"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
         <v>14.8</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>0.01</v>
       </c>
       <c r="D53">
         <v>3</v>
       </c>
-      <c r="E53" s="2">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
         <v>4.6500000000000004</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>0</v>
       </c>
       <c r="D54">
         <v>1.78</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1552,13 +1552,13 @@
       <c r="A55">
         <v>1.84</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>0</v>
       </c>
       <c r="D55">
         <v>0.61799999999999999</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1566,13 +1566,13 @@
       <c r="A56">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="D56">
         <v>0.45600000000000002</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1580,13 +1580,13 @@
       <c r="A57">
         <v>0.247</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>0</v>
       </c>
       <c r="D57">
         <v>0.122</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1594,13 +1594,13 @@
       <c r="A58">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>0</v>
       </c>
       <c r="D58">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1608,13 +1608,13 @@
       <c r="A59">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="D59">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1622,13 +1622,13 @@
       <c r="A60">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>0</v>
       </c>
       <c r="D60">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1636,13 +1636,13 @@
       <c r="A61">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>0</v>
       </c>
       <c r="D61">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1650,13 +1650,13 @@
       <c r="A62">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>0</v>
       </c>
       <c r="D62">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1664,13 +1664,13 @@
       <c r="A63">
         <v>2E-3</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>0</v>
       </c>
       <c r="D63">
         <v>2E-3</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1678,22 +1678,22 @@
       <c r="A64">
         <v>0</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>0</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1701,7 +1701,7 @@
         <f>AVERAGE(A7:A48)</f>
         <v>3035.4047619047619</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <f>AVERAGE(B7:B48)</f>
         <v>4.0395238095238097</v>
       </c>
@@ -1709,19 +1709,19 @@
         <f>AVERAGE(D7:D48)</f>
         <v>1249.5738095238096</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67" s="1">
         <f>AVERAGE(E7:E48)</f>
         <v>1.6957142857142864</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="D69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="D70" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70">
         <f>D67/A67</f>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="D71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E71">
         <f>E67/B67</f>

</xml_diff>